<commit_message>
- Refactor DB_GET_TOP_LEVEL_DATA function and improve style_top_level layout with new Main_info_panel class
</commit_message>
<xml_diff>
--- a/Apparel Merchandisers Helper/DB/top level data.xlsx
+++ b/Apparel Merchandisers Helper/DB/top level data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MyData\learn\Programming\WorkSpace\Apparel-Merchandisers-Helper\Apparel Merchandisers Helper\DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F1ACD4E-9497-4C8E-AD5A-2E5F36FE84D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BEB772E-53D7-48AF-A58C-18629D401044}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>866S</t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t>shipping date</t>
+  </si>
+  <si>
+    <t>GSM</t>
   </si>
 </sst>
 </file>
@@ -228,40 +231,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -559,7 +562,7 @@
   <dimension ref="B1:Y29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="X12" sqref="X12"/>
+      <selection activeCell="Q3" sqref="Q3:R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -568,7 +571,80 @@
     <col min="2" max="30" width="5.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:25" ht="4.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="1" spans="2:25" ht="29.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B1">
+        <v>0</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>2</v>
+      </c>
+      <c r="E1">
+        <v>3</v>
+      </c>
+      <c r="F1">
+        <v>4</v>
+      </c>
+      <c r="G1">
+        <v>5</v>
+      </c>
+      <c r="H1">
+        <v>6</v>
+      </c>
+      <c r="I1">
+        <v>7</v>
+      </c>
+      <c r="J1">
+        <v>8</v>
+      </c>
+      <c r="K1">
+        <v>9</v>
+      </c>
+      <c r="L1">
+        <v>10</v>
+      </c>
+      <c r="M1">
+        <v>11</v>
+      </c>
+      <c r="N1">
+        <v>12</v>
+      </c>
+      <c r="O1">
+        <v>13</v>
+      </c>
+      <c r="P1">
+        <v>14</v>
+      </c>
+      <c r="Q1">
+        <v>15</v>
+      </c>
+      <c r="R1">
+        <v>16</v>
+      </c>
+      <c r="S1">
+        <v>17</v>
+      </c>
+      <c r="T1">
+        <v>18</v>
+      </c>
+      <c r="U1">
+        <v>19</v>
+      </c>
+      <c r="V1">
+        <v>20</v>
+      </c>
+      <c r="W1">
+        <v>21</v>
+      </c>
+      <c r="X1">
+        <v>22</v>
+      </c>
+      <c r="Y1">
+        <v>23</v>
+      </c>
+    </row>
     <row r="2" spans="2:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="16" t="s">
         <v>0</v>
@@ -576,430 +652,432 @@
       <c r="C2" s="17"/>
       <c r="D2" s="17"/>
       <c r="E2" s="17"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6" t="s">
+      <c r="F2" s="1"/>
+      <c r="G2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1" t="s">
+      <c r="I2" s="15"/>
+      <c r="J2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1" t="s">
+      <c r="K2" s="15"/>
+      <c r="L2" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1" t="s">
+      <c r="M2" s="15"/>
+      <c r="N2" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1" t="s">
+      <c r="O2" s="15"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="R2" s="15"/>
+      <c r="S2" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1" t="s">
+      <c r="T2" s="15"/>
+      <c r="U2" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="T2" s="1"/>
-      <c r="U2" s="6"/>
-      <c r="V2" s="2"/>
+      <c r="V2" s="15"/>
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
-      <c r="Y2" s="7"/>
+      <c r="Y2" s="6"/>
     </row>
     <row r="3" spans="2:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="18"/>
       <c r="C3" s="19"/>
       <c r="D3" s="19"/>
       <c r="E3" s="19"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
-      <c r="Q3" s="4"/>
-      <c r="R3" s="4"/>
-      <c r="S3" s="4"/>
-      <c r="T3" s="4"/>
-      <c r="U3" s="8"/>
-      <c r="V3" s="8"/>
-      <c r="W3" s="8"/>
-      <c r="X3" s="8"/>
-      <c r="Y3" s="9"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="11"/>
+      <c r="S3" s="11"/>
+      <c r="T3" s="11"/>
+      <c r="U3" s="11"/>
+      <c r="V3" s="11"/>
+      <c r="W3" s="4"/>
+      <c r="X3" s="4"/>
+      <c r="Y3" s="7"/>
     </row>
     <row r="4" spans="2:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="18"/>
       <c r="C4" s="19"/>
       <c r="D4" s="19"/>
       <c r="E4" s="19"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
-      <c r="P4" s="4"/>
-      <c r="Q4" s="4"/>
-      <c r="R4" s="4"/>
-      <c r="S4" s="4"/>
-      <c r="T4" s="4"/>
-      <c r="U4" s="8"/>
-      <c r="V4" s="8"/>
-      <c r="W4" s="8"/>
-      <c r="X4" s="8"/>
-      <c r="Y4" s="9"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="11"/>
+      <c r="Q4" s="11"/>
+      <c r="R4" s="11"/>
+      <c r="S4" s="11"/>
+      <c r="T4" s="11"/>
+      <c r="U4" s="11"/>
+      <c r="V4" s="11"/>
+      <c r="W4" s="4"/>
+      <c r="X4" s="4"/>
+      <c r="Y4" s="7"/>
     </row>
     <row r="5" spans="2:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="8"/>
-      <c r="O5" s="8"/>
-      <c r="P5" s="8"/>
-      <c r="Q5" s="8"/>
-      <c r="R5" s="8"/>
-      <c r="S5" s="8"/>
-      <c r="T5" s="8"/>
-      <c r="U5" s="8"/>
-      <c r="V5" s="8"/>
-      <c r="W5" s="8"/>
-      <c r="X5" s="8"/>
-      <c r="Y5" s="9"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4"/>
+      <c r="R5" s="4"/>
+      <c r="S5" s="4"/>
+      <c r="T5" s="4"/>
+      <c r="U5" s="4"/>
+      <c r="V5" s="4"/>
+      <c r="W5" s="4"/>
+      <c r="X5" s="4"/>
+      <c r="Y5" s="7"/>
     </row>
     <row r="6" spans="2:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="8" t="s">
+      <c r="C6" s="11"/>
+      <c r="D6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4" t="s">
+      <c r="F6" s="11"/>
+      <c r="G6" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4" t="s">
+      <c r="H6" s="11"/>
+      <c r="I6" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4" t="s">
+      <c r="J6" s="11"/>
+      <c r="K6" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4" t="s">
+      <c r="L6" s="11"/>
+      <c r="M6" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4" t="s">
+      <c r="N6" s="11"/>
+      <c r="O6" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="P6" s="4"/>
-      <c r="Q6" s="4" t="s">
+      <c r="P6" s="11"/>
+      <c r="Q6" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="R6" s="4"/>
-      <c r="S6" s="4" t="s">
+      <c r="R6" s="11"/>
+      <c r="S6" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="T6" s="4"/>
-      <c r="U6" s="4" t="s">
+      <c r="T6" s="11"/>
+      <c r="U6" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="V6" s="4"/>
-      <c r="W6" s="4" t="s">
+      <c r="V6" s="11"/>
+      <c r="W6" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="X6" s="4"/>
+      <c r="X6" s="11"/>
       <c r="Y6" s="5"/>
     </row>
     <row r="7" spans="2:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="3"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
-      <c r="P7" s="4"/>
-      <c r="Q7" s="4"/>
-      <c r="R7" s="4"/>
-      <c r="S7" s="4"/>
-      <c r="T7" s="4"/>
-      <c r="U7" s="4"/>
-      <c r="V7" s="4"/>
-      <c r="W7" s="4"/>
-      <c r="X7" s="4"/>
-      <c r="Y7" s="9"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="11"/>
+      <c r="O7" s="11"/>
+      <c r="P7" s="11"/>
+      <c r="Q7" s="11"/>
+      <c r="R7" s="11"/>
+      <c r="S7" s="11"/>
+      <c r="T7" s="11"/>
+      <c r="U7" s="11"/>
+      <c r="V7" s="11"/>
+      <c r="W7" s="11"/>
+      <c r="X7" s="11"/>
+      <c r="Y7" s="7"/>
     </row>
     <row r="8" spans="2:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="3"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
-      <c r="P8" s="4"/>
-      <c r="Q8" s="4"/>
-      <c r="R8" s="4"/>
-      <c r="S8" s="4"/>
-      <c r="T8" s="4"/>
-      <c r="U8" s="4"/>
-      <c r="V8" s="4"/>
-      <c r="W8" s="4"/>
-      <c r="X8" s="4"/>
-      <c r="Y8" s="9"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="11"/>
+      <c r="P8" s="11"/>
+      <c r="Q8" s="11"/>
+      <c r="R8" s="11"/>
+      <c r="S8" s="11"/>
+      <c r="T8" s="11"/>
+      <c r="U8" s="11"/>
+      <c r="V8" s="11"/>
+      <c r="W8" s="11"/>
+      <c r="X8" s="11"/>
+      <c r="Y8" s="7"/>
     </row>
     <row r="9" spans="2:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="3"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
-      <c r="O9" s="4"/>
-      <c r="P9" s="4"/>
-      <c r="Q9" s="4"/>
-      <c r="R9" s="4"/>
-      <c r="S9" s="4"/>
-      <c r="T9" s="4"/>
-      <c r="U9" s="4"/>
-      <c r="V9" s="4"/>
-      <c r="W9" s="4"/>
-      <c r="X9" s="4"/>
-      <c r="Y9" s="9"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="11"/>
+      <c r="O9" s="11"/>
+      <c r="P9" s="11"/>
+      <c r="Q9" s="11"/>
+      <c r="R9" s="11"/>
+      <c r="S9" s="11"/>
+      <c r="T9" s="11"/>
+      <c r="U9" s="11"/>
+      <c r="V9" s="11"/>
+      <c r="W9" s="11"/>
+      <c r="X9" s="11"/>
+      <c r="Y9" s="7"/>
     </row>
     <row r="10" spans="2:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="10"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
-      <c r="M10" s="8"/>
-      <c r="N10" s="8"/>
-      <c r="O10" s="8"/>
-      <c r="P10" s="8"/>
-      <c r="Q10" s="8"/>
-      <c r="R10" s="8"/>
-      <c r="S10" s="8"/>
-      <c r="T10" s="8"/>
-      <c r="U10" s="8"/>
-      <c r="V10" s="8"/>
-      <c r="W10" s="8"/>
-      <c r="X10" s="8"/>
-      <c r="Y10" s="9"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4"/>
+      <c r="P10" s="4"/>
+      <c r="Q10" s="4"/>
+      <c r="R10" s="4"/>
+      <c r="S10" s="4"/>
+      <c r="T10" s="4"/>
+      <c r="U10" s="4"/>
+      <c r="V10" s="4"/>
+      <c r="W10" s="4"/>
+      <c r="X10" s="4"/>
+      <c r="Y10" s="7"/>
     </row>
     <row r="11" spans="2:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="10"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
-      <c r="M11" s="8"/>
-      <c r="N11" s="8"/>
-      <c r="O11" s="8"/>
-      <c r="P11" s="8"/>
-      <c r="Q11" s="8"/>
-      <c r="R11" s="8"/>
-      <c r="S11" s="8"/>
-      <c r="T11" s="8"/>
-      <c r="U11" s="8"/>
-      <c r="V11" s="8"/>
-      <c r="W11" s="8"/>
-      <c r="X11" s="8"/>
-      <c r="Y11" s="9"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4"/>
+      <c r="O11" s="4"/>
+      <c r="P11" s="4"/>
+      <c r="Q11" s="4"/>
+      <c r="R11" s="4"/>
+      <c r="S11" s="4"/>
+      <c r="T11" s="4"/>
+      <c r="U11" s="4"/>
+      <c r="V11" s="4"/>
+      <c r="W11" s="4"/>
+      <c r="X11" s="4"/>
+      <c r="Y11" s="7"/>
     </row>
     <row r="12" spans="2:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="10"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8"/>
-      <c r="M12" s="8"/>
-      <c r="N12" s="8"/>
-      <c r="O12" s="8"/>
-      <c r="P12" s="8"/>
-      <c r="Q12" s="8"/>
-      <c r="R12" s="8"/>
-      <c r="S12" s="8"/>
-      <c r="T12" s="8"/>
-      <c r="U12" s="8"/>
-      <c r="V12" s="8"/>
-      <c r="W12" s="8"/>
-      <c r="X12" s="8"/>
-      <c r="Y12" s="9"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+      <c r="P12" s="4"/>
+      <c r="Q12" s="4"/>
+      <c r="R12" s="4"/>
+      <c r="S12" s="4"/>
+      <c r="T12" s="4"/>
+      <c r="U12" s="4"/>
+      <c r="V12" s="4"/>
+      <c r="W12" s="4"/>
+      <c r="X12" s="4"/>
+      <c r="Y12" s="7"/>
     </row>
     <row r="13" spans="2:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="10"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="8"/>
-      <c r="M13" s="8"/>
-      <c r="N13" s="8"/>
-      <c r="O13" s="8"/>
-      <c r="P13" s="8"/>
-      <c r="Q13" s="8"/>
-      <c r="R13" s="8"/>
-      <c r="S13" s="8"/>
-      <c r="T13" s="8"/>
-      <c r="U13" s="8"/>
-      <c r="V13" s="8"/>
-      <c r="W13" s="8"/>
-      <c r="X13" s="8"/>
-      <c r="Y13" s="9"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="4"/>
+      <c r="R13" s="4"/>
+      <c r="S13" s="4"/>
+      <c r="T13" s="4"/>
+      <c r="U13" s="4"/>
+      <c r="V13" s="4"/>
+      <c r="W13" s="4"/>
+      <c r="X13" s="4"/>
+      <c r="Y13" s="7"/>
     </row>
     <row r="14" spans="2:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="10"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
-      <c r="L14" s="8"/>
-      <c r="M14" s="8"/>
-      <c r="N14" s="8"/>
-      <c r="O14" s="8"/>
-      <c r="P14" s="8"/>
-      <c r="Q14" s="8"/>
-      <c r="R14" s="8"/>
-      <c r="S14" s="8"/>
-      <c r="T14" s="8"/>
-      <c r="U14" s="8"/>
-      <c r="V14" s="8"/>
-      <c r="W14" s="8"/>
-      <c r="X14" s="8"/>
-      <c r="Y14" s="9"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="4"/>
+      <c r="O14" s="4"/>
+      <c r="P14" s="4"/>
+      <c r="Q14" s="4"/>
+      <c r="R14" s="4"/>
+      <c r="S14" s="4"/>
+      <c r="T14" s="4"/>
+      <c r="U14" s="4"/>
+      <c r="V14" s="4"/>
+      <c r="W14" s="4"/>
+      <c r="X14" s="4"/>
+      <c r="Y14" s="7"/>
     </row>
     <row r="15" spans="2:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="10"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="8"/>
-      <c r="M15" s="8"/>
-      <c r="N15" s="8"/>
-      <c r="O15" s="8"/>
-      <c r="P15" s="8"/>
-      <c r="Q15" s="8"/>
-      <c r="R15" s="8"/>
-      <c r="S15" s="8"/>
-      <c r="T15" s="8"/>
-      <c r="U15" s="8"/>
-      <c r="V15" s="8"/>
-      <c r="W15" s="8"/>
-      <c r="X15" s="8"/>
-      <c r="Y15" s="9"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="4"/>
+      <c r="O15" s="4"/>
+      <c r="P15" s="4"/>
+      <c r="Q15" s="4"/>
+      <c r="R15" s="4"/>
+      <c r="S15" s="4"/>
+      <c r="T15" s="4"/>
+      <c r="U15" s="4"/>
+      <c r="V15" s="4"/>
+      <c r="W15" s="4"/>
+      <c r="X15" s="4"/>
+      <c r="Y15" s="7"/>
     </row>
     <row r="16" spans="2:25" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="11"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
-      <c r="K16" s="12"/>
-      <c r="L16" s="12"/>
-      <c r="M16" s="12"/>
-      <c r="N16" s="12"/>
-      <c r="O16" s="12"/>
-      <c r="P16" s="12"/>
-      <c r="Q16" s="12"/>
-      <c r="R16" s="12"/>
-      <c r="S16" s="12"/>
-      <c r="T16" s="12"/>
-      <c r="U16" s="12"/>
-      <c r="V16" s="12"/>
-      <c r="W16" s="12"/>
-      <c r="X16" s="12"/>
-      <c r="Y16" s="13"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="9"/>
+      <c r="O16" s="9"/>
+      <c r="P16" s="9"/>
+      <c r="Q16" s="9"/>
+      <c r="R16" s="9"/>
+      <c r="S16" s="9"/>
+      <c r="T16" s="9"/>
+      <c r="U16" s="9"/>
+      <c r="V16" s="9"/>
+      <c r="W16" s="9"/>
+      <c r="X16" s="9"/>
+      <c r="Y16" s="10"/>
     </row>
     <row r="17" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="18" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1015,21 +1093,36 @@
     <row r="28" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="29" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <mergeCells count="49">
-    <mergeCell ref="S7:T9"/>
-    <mergeCell ref="U6:V6"/>
-    <mergeCell ref="U7:V9"/>
-    <mergeCell ref="W6:X6"/>
-    <mergeCell ref="W7:X9"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="O7:P7"/>
-    <mergeCell ref="O8:P8"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="Q6:R6"/>
-    <mergeCell ref="S6:T6"/>
-    <mergeCell ref="Q7:R7"/>
-    <mergeCell ref="Q8:R8"/>
-    <mergeCell ref="Q9:R9"/>
+  <mergeCells count="51">
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="U3:V4"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="B2:E4"/>
+    <mergeCell ref="H3:I4"/>
+    <mergeCell ref="J3:K4"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="N3:P4"/>
+    <mergeCell ref="Q3:R4"/>
+    <mergeCell ref="S3:T4"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="N2:P2"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="E7:F9"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C9"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="G7:H9"/>
     <mergeCell ref="K6:L6"/>
     <mergeCell ref="M6:N6"/>
     <mergeCell ref="K7:L7"/>
@@ -1038,33 +1131,20 @@
     <mergeCell ref="M7:N7"/>
     <mergeCell ref="M8:N8"/>
     <mergeCell ref="M9:N9"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="G7:H9"/>
-    <mergeCell ref="E7:F9"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C9"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="N3:P4"/>
-    <mergeCell ref="Q3:R4"/>
-    <mergeCell ref="S3:T4"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="N2:P2"/>
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="B2:E4"/>
-    <mergeCell ref="H3:I4"/>
-    <mergeCell ref="J3:K4"/>
-    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="Q6:R6"/>
+    <mergeCell ref="Q7:R7"/>
+    <mergeCell ref="Q8:R8"/>
+    <mergeCell ref="Q9:R9"/>
+    <mergeCell ref="S7:T9"/>
+    <mergeCell ref="U6:V6"/>
+    <mergeCell ref="U7:V9"/>
+    <mergeCell ref="W6:X6"/>
+    <mergeCell ref="W7:X9"/>
+    <mergeCell ref="S6:T6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Refactor price field in DB_GET_TOP_LEVEL_DATA and finish Main info panel for top level and progress  with Po_data_panel class
</commit_message>
<xml_diff>
--- a/Apparel Merchandisers Helper/DB/top level data.xlsx
+++ b/Apparel Merchandisers Helper/DB/top level data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MyData\learn\Programming\WorkSpace\Apparel-Merchandisers-Helper\Apparel Merchandisers Helper\DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BEB772E-53D7-48AF-A58C-18629D401044}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB3A6923-0B99-4CF0-814D-8F6D3AF69390}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -252,9 +252,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -262,21 +277,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -559,19 +559,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:Y29"/>
+  <dimension ref="A1:Y29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3:R4"/>
+      <selection activeCell="S7" sqref="S7:T9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="0.88671875" customWidth="1"/>
+    <col min="1" max="1" width="6.109375" customWidth="1"/>
     <col min="2" max="30" width="5.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:25" ht="29.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:25" ht="29.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1">
         <v>0</v>
       </c>
@@ -645,109 +645,112 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="2:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="16" t="s">
+    <row r="2" spans="1:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="H2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15" t="s">
+      <c r="I2" s="11"/>
+      <c r="J2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15" t="s">
+      <c r="K2" s="11"/>
+      <c r="L2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="M2" s="15"/>
-      <c r="N2" s="15" t="s">
+      <c r="M2" s="11"/>
+      <c r="N2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="15"/>
-      <c r="P2" s="15"/>
-      <c r="Q2" s="15" t="s">
+      <c r="O2" s="11"/>
+      <c r="P2" s="11"/>
+      <c r="Q2" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="R2" s="15"/>
-      <c r="S2" s="15" t="s">
+      <c r="R2" s="11"/>
+      <c r="S2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="T2" s="15"/>
-      <c r="U2" s="15" t="s">
+      <c r="T2" s="11"/>
+      <c r="U2" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="V2" s="15"/>
+      <c r="V2" s="11"/>
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
       <c r="Y2" s="6"/>
     </row>
-    <row r="3" spans="2:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="18"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
+    <row r="3" spans="1:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="15"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
       <c r="F3" s="4"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
-      <c r="M3" s="11"/>
-      <c r="N3" s="11"/>
-      <c r="O3" s="11"/>
-      <c r="P3" s="11"/>
-      <c r="Q3" s="11"/>
-      <c r="R3" s="11"/>
-      <c r="S3" s="11"/>
-      <c r="T3" s="11"/>
-      <c r="U3" s="11"/>
-      <c r="V3" s="11"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="12"/>
+      <c r="N3" s="12"/>
+      <c r="O3" s="12"/>
+      <c r="P3" s="12"/>
+      <c r="Q3" s="12"/>
+      <c r="R3" s="12"/>
+      <c r="S3" s="12"/>
+      <c r="T3" s="12"/>
+      <c r="U3" s="12"/>
+      <c r="V3" s="12"/>
       <c r="W3" s="4"/>
       <c r="X3" s="4"/>
       <c r="Y3" s="7"/>
     </row>
-    <row r="4" spans="2:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="18"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
+    <row r="4" spans="1:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="15"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
       <c r="F4" s="4"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="11"/>
-      <c r="N4" s="11"/>
-      <c r="O4" s="11"/>
-      <c r="P4" s="11"/>
-      <c r="Q4" s="11"/>
-      <c r="R4" s="11"/>
-      <c r="S4" s="11"/>
-      <c r="T4" s="11"/>
-      <c r="U4" s="11"/>
-      <c r="V4" s="11"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="12"/>
+      <c r="O4" s="12"/>
+      <c r="P4" s="12"/>
+      <c r="Q4" s="12"/>
+      <c r="R4" s="12"/>
+      <c r="S4" s="12"/>
+      <c r="T4" s="12"/>
+      <c r="U4" s="12"/>
+      <c r="V4" s="12"/>
       <c r="W4" s="4"/>
       <c r="X4" s="4"/>
       <c r="Y4" s="7"/>
     </row>
-    <row r="5" spans="2:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="12" t="s">
+    <row r="5" spans="1:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
@@ -769,135 +772,147 @@
       <c r="X5" s="4"/>
       <c r="Y5" s="7"/>
     </row>
-    <row r="6" spans="2:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="14" t="s">
+    <row r="6" spans="1:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="11"/>
+      <c r="C6" s="12"/>
       <c r="D6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E6" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11" t="s">
+      <c r="F6" s="12"/>
+      <c r="G6" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11" t="s">
+      <c r="H6" s="12"/>
+      <c r="I6" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11" t="s">
+      <c r="J6" s="12"/>
+      <c r="K6" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="L6" s="11"/>
-      <c r="M6" s="11" t="s">
+      <c r="L6" s="12"/>
+      <c r="M6" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="N6" s="11"/>
-      <c r="O6" s="11" t="s">
+      <c r="N6" s="12"/>
+      <c r="O6" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="P6" s="11"/>
-      <c r="Q6" s="11" t="s">
+      <c r="P6" s="12"/>
+      <c r="Q6" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="R6" s="11"/>
-      <c r="S6" s="11" t="s">
+      <c r="R6" s="12"/>
+      <c r="S6" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="T6" s="11"/>
-      <c r="U6" s="11" t="s">
+      <c r="T6" s="12"/>
+      <c r="U6" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="V6" s="11"/>
-      <c r="W6" s="11" t="s">
+      <c r="V6" s="12"/>
+      <c r="W6" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="X6" s="11"/>
+      <c r="X6" s="12"/>
       <c r="Y6" s="5"/>
     </row>
-    <row r="7" spans="2:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="14"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="11"/>
-      <c r="L7" s="11"/>
-      <c r="M7" s="11"/>
-      <c r="N7" s="11"/>
-      <c r="O7" s="11"/>
-      <c r="P7" s="11"/>
-      <c r="Q7" s="11"/>
-      <c r="R7" s="11"/>
-      <c r="S7" s="11"/>
-      <c r="T7" s="11"/>
-      <c r="U7" s="11"/>
-      <c r="V7" s="11"/>
-      <c r="W7" s="11"/>
-      <c r="X7" s="11"/>
+    <row r="7" spans="1:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7" s="19"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="12"/>
+      <c r="N7" s="12"/>
+      <c r="O7" s="12"/>
+      <c r="P7" s="12"/>
+      <c r="Q7" s="12"/>
+      <c r="R7" s="12"/>
+      <c r="S7" s="12"/>
+      <c r="T7" s="12"/>
+      <c r="U7" s="12"/>
+      <c r="V7" s="12"/>
+      <c r="W7" s="12"/>
+      <c r="X7" s="12"/>
       <c r="Y7" s="7"/>
     </row>
-    <row r="8" spans="2:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="14"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="11"/>
-      <c r="L8" s="11"/>
-      <c r="M8" s="11"/>
-      <c r="N8" s="11"/>
-      <c r="O8" s="11"/>
-      <c r="P8" s="11"/>
-      <c r="Q8" s="11"/>
-      <c r="R8" s="11"/>
-      <c r="S8" s="11"/>
-      <c r="T8" s="11"/>
-      <c r="U8" s="11"/>
-      <c r="V8" s="11"/>
-      <c r="W8" s="11"/>
-      <c r="X8" s="11"/>
+    <row r="8" spans="1:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8" s="19"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
+      <c r="N8" s="12"/>
+      <c r="O8" s="12"/>
+      <c r="P8" s="12"/>
+      <c r="Q8" s="12"/>
+      <c r="R8" s="12"/>
+      <c r="S8" s="12"/>
+      <c r="T8" s="12"/>
+      <c r="U8" s="12"/>
+      <c r="V8" s="12"/>
+      <c r="W8" s="12"/>
+      <c r="X8" s="12"/>
       <c r="Y8" s="7"/>
     </row>
-    <row r="9" spans="2:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="14"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="11"/>
-      <c r="L9" s="11"/>
-      <c r="M9" s="11"/>
-      <c r="N9" s="11"/>
-      <c r="O9" s="11"/>
-      <c r="P9" s="11"/>
-      <c r="Q9" s="11"/>
-      <c r="R9" s="11"/>
-      <c r="S9" s="11"/>
-      <c r="T9" s="11"/>
-      <c r="U9" s="11"/>
-      <c r="V9" s="11"/>
-      <c r="W9" s="11"/>
-      <c r="X9" s="11"/>
+    <row r="9" spans="1:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>4</v>
+      </c>
+      <c r="B9" s="19"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="12"/>
+      <c r="N9" s="12"/>
+      <c r="O9" s="12"/>
+      <c r="P9" s="12"/>
+      <c r="Q9" s="12"/>
+      <c r="R9" s="12"/>
+      <c r="S9" s="12"/>
+      <c r="T9" s="12"/>
+      <c r="U9" s="12"/>
+      <c r="V9" s="12"/>
+      <c r="W9" s="12"/>
+      <c r="X9" s="12"/>
       <c r="Y9" s="7"/>
     </row>
-    <row r="10" spans="2:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="3"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
@@ -923,7 +938,7 @@
       <c r="X10" s="4"/>
       <c r="Y10" s="7"/>
     </row>
-    <row r="11" spans="2:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="3"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
@@ -949,7 +964,7 @@
       <c r="X11" s="4"/>
       <c r="Y11" s="7"/>
     </row>
-    <row r="12" spans="2:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="3"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
@@ -975,7 +990,7 @@
       <c r="X12" s="4"/>
       <c r="Y12" s="7"/>
     </row>
-    <row r="13" spans="2:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="3"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
@@ -1001,7 +1016,7 @@
       <c r="X13" s="4"/>
       <c r="Y13" s="7"/>
     </row>
-    <row r="14" spans="2:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="3"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
@@ -1027,7 +1042,7 @@
       <c r="X14" s="4"/>
       <c r="Y14" s="7"/>
     </row>
-    <row r="15" spans="2:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="3"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
@@ -1053,7 +1068,7 @@
       <c r="X15" s="4"/>
       <c r="Y15" s="7"/>
     </row>
-    <row r="16" spans="2:25" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:25" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="8"/>
       <c r="C16" s="9"/>
       <c r="D16" s="9"/>
@@ -1094,22 +1109,33 @@
     <row r="29" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="51">
-    <mergeCell ref="U2:V2"/>
-    <mergeCell ref="U3:V4"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="B2:E4"/>
-    <mergeCell ref="H3:I4"/>
-    <mergeCell ref="J3:K4"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="N3:P4"/>
-    <mergeCell ref="Q3:R4"/>
-    <mergeCell ref="S3:T4"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="N2:P2"/>
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="S7:T9"/>
+    <mergeCell ref="U6:V6"/>
+    <mergeCell ref="U7:V9"/>
+    <mergeCell ref="W6:X6"/>
+    <mergeCell ref="W7:X9"/>
+    <mergeCell ref="S6:T6"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="Q6:R6"/>
+    <mergeCell ref="Q7:R7"/>
+    <mergeCell ref="Q8:R8"/>
+    <mergeCell ref="Q9:R9"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="G7:H9"/>
     <mergeCell ref="E7:F9"/>
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="B5:E5"/>
@@ -1118,33 +1144,22 @@
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="G6:H6"/>
     <mergeCell ref="D7:D9"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="G7:H9"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="O7:P7"/>
-    <mergeCell ref="O8:P8"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="Q6:R6"/>
-    <mergeCell ref="Q7:R7"/>
-    <mergeCell ref="Q8:R8"/>
-    <mergeCell ref="Q9:R9"/>
-    <mergeCell ref="S7:T9"/>
-    <mergeCell ref="U6:V6"/>
-    <mergeCell ref="U7:V9"/>
-    <mergeCell ref="W6:X6"/>
-    <mergeCell ref="W7:X9"/>
-    <mergeCell ref="S6:T6"/>
+    <mergeCell ref="B2:E4"/>
+    <mergeCell ref="H3:I4"/>
+    <mergeCell ref="J3:K4"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="N3:P4"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="N2:P2"/>
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="U3:V4"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="Q3:R4"/>
+    <mergeCell ref="S3:T4"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="S2:T2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>